<commit_message>
j'ai corriger les regles qui ne marchait pas
</commit_message>
<xml_diff>
--- a/app/projet/src/main/resources/app/Tableur.xlsx
+++ b/app/projet/src/main/resources/app/Tableur.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nadir\Desktop\2024_2025\S1\GL\Projet\Syllogism\app\projet\src\main\resources\app\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0DCB9DB-D121-4CDC-B52E-868E6111807C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD612CDE-8047-4741-B781-A8C9228697DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="11625" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -386,8 +386,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75DF87F3-69BE-4A64-BC3C-68D3122079E6}">
   <dimension ref="A1:O256"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A239" workbookViewId="0">
-      <selection activeCell="K6" sqref="K6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -6437,7 +6437,7 @@
         <v>1</v>
       </c>
       <c r="J129" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K129" t="b">
         <v>0</v>
@@ -7941,7 +7941,7 @@
         <v>1</v>
       </c>
       <c r="J161" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K161" t="b">
         <v>0</v>
@@ -9445,7 +9445,7 @@
         <v>1</v>
       </c>
       <c r="J193" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K193" t="b">
         <v>0</v>
@@ -10949,7 +10949,7 @@
         <v>1</v>
       </c>
       <c r="J225" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K225" t="b">
         <v>0</v>
@@ -12430,6 +12430,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="8769bae9-3463-4a10-a579-45503be70aed" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="8dfbc409-28c6-489e-afb0-89cc2b931f2a">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101008CB9B2C0AF3CE84CB4250F7CDCA74D24" ma:contentTypeVersion="11" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="2f42a97d5ab0c3bd2930341450d6f06b">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="8dfbc409-28c6-489e-afb0-89cc2b931f2a" xmlns:ns3="8769bae9-3463-4a10-a579-45503be70aed" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="dbd40f3811e35be07f3bce4a65cfcd28" ns2:_="" ns3:_="">
     <xsd:import namespace="8dfbc409-28c6-489e-afb0-89cc2b931f2a"/>
@@ -12624,27 +12644,26 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AFBD511E-5C1D-4223-BB26-D22E6EE722D3}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="8769bae9-3463-4a10-a579-45503be70aed"/>
+    <ds:schemaRef ds:uri="8dfbc409-28c6-489e-afb0-89cc2b931f2a"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="8769bae9-3463-4a10-a579-45503be70aed" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="8dfbc409-28c6-489e-afb0-89cc2b931f2a">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CE0CAF50-C050-48AE-875E-A3DE6E22B7B5}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EE972C20-CF49-42CA-B59D-0D1129D9A052}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -12661,23 +12680,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CE0CAF50-C050-48AE-875E-A3DE6E22B7B5}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AFBD511E-5C1D-4223-BB26-D22E6EE722D3}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="8769bae9-3463-4a10-a579-45503be70aed"/>
-    <ds:schemaRef ds:uri="8dfbc409-28c6-489e-afb0-89cc2b931f2a"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
j'ai corriger les regles qui ne marchait pas (#12)
</commit_message>
<xml_diff>
--- a/app/projet/src/main/resources/app/Tableur.xlsx
+++ b/app/projet/src/main/resources/app/Tableur.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nadir\Desktop\2024_2025\S1\GL\Projet\Syllogism\app\projet\src\main\resources\app\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0DCB9DB-D121-4CDC-B52E-868E6111807C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD612CDE-8047-4741-B781-A8C9228697DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="11625" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -386,8 +386,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75DF87F3-69BE-4A64-BC3C-68D3122079E6}">
   <dimension ref="A1:O256"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A239" workbookViewId="0">
-      <selection activeCell="K6" sqref="K6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -6437,7 +6437,7 @@
         <v>1</v>
       </c>
       <c r="J129" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K129" t="b">
         <v>0</v>
@@ -7941,7 +7941,7 @@
         <v>1</v>
       </c>
       <c r="J161" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K161" t="b">
         <v>0</v>
@@ -9445,7 +9445,7 @@
         <v>1</v>
       </c>
       <c r="J193" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K193" t="b">
         <v>0</v>
@@ -10949,7 +10949,7 @@
         <v>1</v>
       </c>
       <c r="J225" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K225" t="b">
         <v>0</v>
@@ -12430,6 +12430,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="8769bae9-3463-4a10-a579-45503be70aed" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="8dfbc409-28c6-489e-afb0-89cc2b931f2a">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101008CB9B2C0AF3CE84CB4250F7CDCA74D24" ma:contentTypeVersion="11" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="2f42a97d5ab0c3bd2930341450d6f06b">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="8dfbc409-28c6-489e-afb0-89cc2b931f2a" xmlns:ns3="8769bae9-3463-4a10-a579-45503be70aed" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="dbd40f3811e35be07f3bce4a65cfcd28" ns2:_="" ns3:_="">
     <xsd:import namespace="8dfbc409-28c6-489e-afb0-89cc2b931f2a"/>
@@ -12624,27 +12644,26 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AFBD511E-5C1D-4223-BB26-D22E6EE722D3}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="8769bae9-3463-4a10-a579-45503be70aed"/>
+    <ds:schemaRef ds:uri="8dfbc409-28c6-489e-afb0-89cc2b931f2a"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="8769bae9-3463-4a10-a579-45503be70aed" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="8dfbc409-28c6-489e-afb0-89cc2b931f2a">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CE0CAF50-C050-48AE-875E-A3DE6E22B7B5}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EE972C20-CF49-42CA-B59D-0D1129D9A052}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -12661,23 +12680,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CE0CAF50-C050-48AE-875E-A3DE6E22B7B5}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AFBD511E-5C1D-4223-BB26-D22E6EE722D3}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="8769bae9-3463-4a10-a579-45503be70aed"/>
-    <ds:schemaRef ds:uri="8dfbc409-28c6-489e-afb0-89cc2b931f2a"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
filter array + small fix(#43)
</commit_message>
<xml_diff>
--- a/app/projet/src/main/resources/app/Tableur.xlsx
+++ b/app/projet/src/main/resources/app/Tableur.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nadir\Desktop\2024_2025\S1\GL\Projet\Syllogism\app\projet\src\main\resources\app\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://etuunivpoitiersfr-my.sharepoint.com/personal/nathanael_maitrehenry_etu_univ-poitiers_fr/Documents/Documents Fac/fac/M1/GL/Syllogism/app/projet/src/main/resources/app/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD612CDE-8047-4741-B781-A8C9228697DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="10" documentId="13_ncr:1_{AD612CDE-8047-4741-B781-A8C9228697DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5CCA85E1-0504-4403-8794-A6CFC0CE5FBA}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="11625" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="780" yWindow="705" windowWidth="28020" windowHeight="14775" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="2" r:id="rId1"/>
@@ -97,6 +97,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -387,12 +391,12 @@
   <dimension ref="A1:O256"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+      <selection activeCell="O259" sqref="O259"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -439,7 +443,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -486,7 +490,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -533,7 +537,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -580,7 +584,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>0</v>
       </c>
@@ -627,7 +631,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>0</v>
       </c>
@@ -674,7 +678,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>0</v>
       </c>
@@ -721,7 +725,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>0</v>
       </c>
@@ -768,7 +772,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>0</v>
       </c>
@@ -815,7 +819,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>0</v>
       </c>
@@ -862,7 +866,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>0</v>
       </c>
@@ -906,10 +910,10 @@
         <v>1</v>
       </c>
       <c r="O11" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>0</v>
       </c>
@@ -953,10 +957,10 @@
         <v>1</v>
       </c>
       <c r="O12" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>0</v>
       </c>
@@ -1003,7 +1007,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>0</v>
       </c>
@@ -1050,7 +1054,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>0</v>
       </c>
@@ -1097,7 +1101,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>0</v>
       </c>
@@ -1144,7 +1148,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>0</v>
       </c>
@@ -1191,7 +1195,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>0</v>
       </c>
@@ -1238,7 +1242,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>0</v>
       </c>
@@ -1285,7 +1289,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>0</v>
       </c>
@@ -1332,7 +1336,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>0</v>
       </c>
@@ -1379,7 +1383,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>0</v>
       </c>
@@ -1426,7 +1430,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>0</v>
       </c>
@@ -1473,7 +1477,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>0</v>
       </c>
@@ -1520,7 +1524,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>0</v>
       </c>
@@ -1567,7 +1571,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>0</v>
       </c>
@@ -1614,7 +1618,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>0</v>
       </c>
@@ -1661,7 +1665,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>0</v>
       </c>
@@ -1708,7 +1712,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>0</v>
       </c>
@@ -1755,7 +1759,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>0</v>
       </c>
@@ -1802,7 +1806,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>0</v>
       </c>
@@ -1849,7 +1853,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>0</v>
       </c>
@@ -1893,10 +1897,10 @@
         <v>1</v>
       </c>
       <c r="O32" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>0</v>
       </c>
@@ -1943,7 +1947,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>0</v>
       </c>
@@ -1990,7 +1994,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>0</v>
       </c>
@@ -2037,7 +2041,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>0</v>
       </c>
@@ -2084,7 +2088,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>0</v>
       </c>
@@ -2131,7 +2135,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>0</v>
       </c>
@@ -2178,7 +2182,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>0</v>
       </c>
@@ -2225,7 +2229,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>0</v>
       </c>
@@ -2272,7 +2276,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>0</v>
       </c>
@@ -2319,7 +2323,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>0</v>
       </c>
@@ -2366,7 +2370,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>0</v>
       </c>
@@ -2413,7 +2417,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>0</v>
       </c>
@@ -2460,7 +2464,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>0</v>
       </c>
@@ -2507,7 +2511,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>0</v>
       </c>
@@ -2554,7 +2558,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>0</v>
       </c>
@@ -2601,7 +2605,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>0</v>
       </c>
@@ -2648,7 +2652,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>0</v>
       </c>
@@ -2695,7 +2699,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>0</v>
       </c>
@@ -2742,7 +2746,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>0</v>
       </c>
@@ -2789,7 +2793,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>0</v>
       </c>
@@ -2836,7 +2840,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>0</v>
       </c>
@@ -2883,7 +2887,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>0</v>
       </c>
@@ -2930,7 +2934,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>0</v>
       </c>
@@ -2977,7 +2981,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>0</v>
       </c>
@@ -3024,7 +3028,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>0</v>
       </c>
@@ -3071,7 +3075,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>0</v>
       </c>
@@ -3118,7 +3122,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>0</v>
       </c>
@@ -3165,7 +3169,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>0</v>
       </c>
@@ -3212,7 +3216,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>0</v>
       </c>
@@ -3259,7 +3263,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>0</v>
       </c>
@@ -3306,7 +3310,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>0</v>
       </c>
@@ -3353,7 +3357,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="64" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>0</v>
       </c>
@@ -3400,7 +3404,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="65" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>1</v>
       </c>
@@ -3447,7 +3451,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="66" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>1</v>
       </c>
@@ -3494,7 +3498,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="67" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>1</v>
       </c>
@@ -3541,7 +3545,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="68" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>1</v>
       </c>
@@ -3588,7 +3592,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="69" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>1</v>
       </c>
@@ -3635,7 +3639,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="70" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>1</v>
       </c>
@@ -3682,7 +3686,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="71" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>1</v>
       </c>
@@ -3729,7 +3733,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="72" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>1</v>
       </c>
@@ -3776,7 +3780,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="73" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>1</v>
       </c>
@@ -3823,7 +3827,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="74" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>1</v>
       </c>
@@ -3870,7 +3874,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="75" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>1</v>
       </c>
@@ -3917,7 +3921,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="76" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>1</v>
       </c>
@@ -3964,7 +3968,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="77" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>1</v>
       </c>
@@ -4011,7 +4015,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="78" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="78" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>1</v>
       </c>
@@ -4058,7 +4062,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="79" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="79" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>1</v>
       </c>
@@ -4102,10 +4106,10 @@
         <v>1</v>
       </c>
       <c r="O79" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="80" spans="1:15" x14ac:dyDescent="0.45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="80" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>1</v>
       </c>
@@ -4149,10 +4153,10 @@
         <v>1</v>
       </c>
       <c r="O80" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="81" spans="1:15" x14ac:dyDescent="0.45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="81" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>1</v>
       </c>
@@ -4199,7 +4203,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="82" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>1</v>
       </c>
@@ -4246,7 +4250,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="83" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>1</v>
       </c>
@@ -4293,7 +4297,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="84" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>1</v>
       </c>
@@ -4340,7 +4344,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="85" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>1</v>
       </c>
@@ -4387,7 +4391,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="86" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>1</v>
       </c>
@@ -4434,7 +4438,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="87" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>1</v>
       </c>
@@ -4481,7 +4485,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="88" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>1</v>
       </c>
@@ -4528,7 +4532,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="89" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>1</v>
       </c>
@@ -4575,7 +4579,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="90" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>1</v>
       </c>
@@ -4622,7 +4626,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="91" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>1</v>
       </c>
@@ -4669,7 +4673,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="92" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>1</v>
       </c>
@@ -4716,7 +4720,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="93" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>1</v>
       </c>
@@ -4763,7 +4767,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="94" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>1</v>
       </c>
@@ -4810,7 +4814,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="95" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>1</v>
       </c>
@@ -4857,7 +4861,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="96" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>1</v>
       </c>
@@ -4904,7 +4908,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="97" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>1</v>
       </c>
@@ -4951,7 +4955,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="98" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>1</v>
       </c>
@@ -4998,7 +5002,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="99" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>1</v>
       </c>
@@ -5045,7 +5049,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="100" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>1</v>
       </c>
@@ -5092,7 +5096,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="101" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="101" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>1</v>
       </c>
@@ -5139,7 +5143,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="102" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="102" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>1</v>
       </c>
@@ -5186,7 +5190,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="103" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="103" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>1</v>
       </c>
@@ -5233,7 +5237,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="104" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="104" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>1</v>
       </c>
@@ -5280,7 +5284,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="105" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="105" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>1</v>
       </c>
@@ -5327,7 +5331,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="106" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="106" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>1</v>
       </c>
@@ -5374,7 +5378,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="107" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="107" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>1</v>
       </c>
@@ -5421,7 +5425,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="108" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="108" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>1</v>
       </c>
@@ -5468,7 +5472,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="109" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="109" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>1</v>
       </c>
@@ -5515,7 +5519,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="110" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="110" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>1</v>
       </c>
@@ -5562,7 +5566,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="111" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="111" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>1</v>
       </c>
@@ -5609,7 +5613,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="112" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="112" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>1</v>
       </c>
@@ -5656,7 +5660,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="113" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="113" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>1</v>
       </c>
@@ -5703,7 +5707,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="114" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="114" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>1</v>
       </c>
@@ -5750,7 +5754,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="115" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="115" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>1</v>
       </c>
@@ -5797,7 +5801,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="116" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="116" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>1</v>
       </c>
@@ -5844,7 +5848,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="117" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="117" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>1</v>
       </c>
@@ -5891,7 +5895,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="118" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="118" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>1</v>
       </c>
@@ -5938,7 +5942,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="119" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="119" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>1</v>
       </c>
@@ -5985,7 +5989,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="120" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="120" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>1</v>
       </c>
@@ -6032,7 +6036,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="121" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="121" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>1</v>
       </c>
@@ -6079,7 +6083,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="122" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="122" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>1</v>
       </c>
@@ -6126,7 +6130,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="123" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="123" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>1</v>
       </c>
@@ -6173,7 +6177,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="124" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="124" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>1</v>
       </c>
@@ -6220,7 +6224,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="125" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="125" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>1</v>
       </c>
@@ -6267,7 +6271,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="126" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="126" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>1</v>
       </c>
@@ -6314,7 +6318,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="127" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="127" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>1</v>
       </c>
@@ -6361,7 +6365,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="128" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="128" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>1</v>
       </c>
@@ -6408,7 +6412,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="129" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="129" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>2</v>
       </c>
@@ -6455,7 +6459,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="130" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="130" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>2</v>
       </c>
@@ -6502,7 +6506,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="131" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="131" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>2</v>
       </c>
@@ -6549,7 +6553,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="132" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="132" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>2</v>
       </c>
@@ -6596,7 +6600,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="133" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="133" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>2</v>
       </c>
@@ -6643,7 +6647,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="134" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="134" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>2</v>
       </c>
@@ -6690,7 +6694,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="135" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="135" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>2</v>
       </c>
@@ -6737,7 +6741,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="136" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="136" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>2</v>
       </c>
@@ -6784,7 +6788,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="137" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="137" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>2</v>
       </c>
@@ -6831,7 +6835,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="138" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="138" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>2</v>
       </c>
@@ -6878,7 +6882,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="139" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="139" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>2</v>
       </c>
@@ -6925,7 +6929,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="140" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="140" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>2</v>
       </c>
@@ -6972,7 +6976,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="141" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="141" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>2</v>
       </c>
@@ -7019,7 +7023,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="142" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="142" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>2</v>
       </c>
@@ -7066,7 +7070,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="143" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="143" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>2</v>
       </c>
@@ -7113,7 +7117,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="144" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="144" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>2</v>
       </c>
@@ -7160,7 +7164,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="145" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="145" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>2</v>
       </c>
@@ -7207,7 +7211,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="146" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="146" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>2</v>
       </c>
@@ -7254,7 +7258,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="147" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="147" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>2</v>
       </c>
@@ -7301,7 +7305,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="148" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="148" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>2</v>
       </c>
@@ -7348,7 +7352,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="149" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="149" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>2</v>
       </c>
@@ -7395,7 +7399,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="150" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="150" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
         <v>2</v>
       </c>
@@ -7442,7 +7446,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="151" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="151" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
         <v>2</v>
       </c>
@@ -7489,7 +7493,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="152" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="152" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
         <v>2</v>
       </c>
@@ -7536,7 +7540,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="153" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="153" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
         <v>2</v>
       </c>
@@ -7583,7 +7587,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="154" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="154" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
         <v>2</v>
       </c>
@@ -7630,7 +7634,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="155" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="155" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
         <v>2</v>
       </c>
@@ -7677,7 +7681,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="156" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="156" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
         <v>2</v>
       </c>
@@ -7724,7 +7728,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="157" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="157" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
         <v>2</v>
       </c>
@@ -7771,7 +7775,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="158" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="158" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
         <v>2</v>
       </c>
@@ -7818,7 +7822,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="159" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="159" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
         <v>2</v>
       </c>
@@ -7865,7 +7869,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="160" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="160" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
         <v>2</v>
       </c>
@@ -7912,7 +7916,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="161" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="161" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
         <v>2</v>
       </c>
@@ -7959,7 +7963,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="162" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="162" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
         <v>2</v>
       </c>
@@ -8006,7 +8010,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="163" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="163" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
         <v>2</v>
       </c>
@@ -8053,7 +8057,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="164" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="164" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
         <v>2</v>
       </c>
@@ -8100,7 +8104,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="165" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="165" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
         <v>2</v>
       </c>
@@ -8147,7 +8151,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="166" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="166" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
         <v>2</v>
       </c>
@@ -8194,7 +8198,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="167" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="167" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
         <v>2</v>
       </c>
@@ -8241,7 +8245,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="168" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="168" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
         <v>2</v>
       </c>
@@ -8288,7 +8292,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="169" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="169" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
         <v>2</v>
       </c>
@@ -8335,7 +8339,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="170" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="170" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
         <v>2</v>
       </c>
@@ -8382,7 +8386,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="171" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="171" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
         <v>2</v>
       </c>
@@ -8429,7 +8433,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="172" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="172" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
         <v>2</v>
       </c>
@@ -8476,7 +8480,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="173" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="173" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
         <v>2</v>
       </c>
@@ -8523,7 +8527,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="174" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="174" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
         <v>2</v>
       </c>
@@ -8570,7 +8574,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="175" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="175" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
         <v>2</v>
       </c>
@@ -8617,7 +8621,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="176" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="176" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
         <v>2</v>
       </c>
@@ -8664,7 +8668,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="177" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="177" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
         <v>2</v>
       </c>
@@ -8711,7 +8715,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="178" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="178" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
         <v>2</v>
       </c>
@@ -8758,7 +8762,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="179" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="179" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
         <v>2</v>
       </c>
@@ -8805,7 +8809,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="180" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="180" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
         <v>2</v>
       </c>
@@ -8852,7 +8856,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="181" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="181" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
         <v>2</v>
       </c>
@@ -8899,7 +8903,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="182" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="182" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
         <v>2</v>
       </c>
@@ -8946,7 +8950,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="183" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="183" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
         <v>2</v>
       </c>
@@ -8993,7 +8997,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="184" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="184" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
         <v>2</v>
       </c>
@@ -9040,7 +9044,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="185" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="185" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
         <v>2</v>
       </c>
@@ -9087,7 +9091,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="186" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="186" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
         <v>2</v>
       </c>
@@ -9134,7 +9138,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="187" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="187" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
         <v>2</v>
       </c>
@@ -9181,7 +9185,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="188" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="188" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
         <v>2</v>
       </c>
@@ -9228,7 +9232,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="189" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="189" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
         <v>2</v>
       </c>
@@ -9275,7 +9279,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="190" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="190" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
         <v>2</v>
       </c>
@@ -9322,7 +9326,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="191" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="191" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
         <v>2</v>
       </c>
@@ -9369,7 +9373,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="192" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="192" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
         <v>2</v>
       </c>
@@ -9416,7 +9420,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="193" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="193" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
         <v>3</v>
       </c>
@@ -9463,7 +9467,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="194" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="194" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
         <v>3</v>
       </c>
@@ -9510,7 +9514,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="195" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="195" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
         <v>3</v>
       </c>
@@ -9557,7 +9561,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="196" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="196" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
         <v>3</v>
       </c>
@@ -9604,7 +9608,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="197" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="197" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
         <v>3</v>
       </c>
@@ -9651,7 +9655,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="198" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="198" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
         <v>3</v>
       </c>
@@ -9698,7 +9702,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="199" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="199" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
         <v>3</v>
       </c>
@@ -9745,7 +9749,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="200" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="200" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
         <v>3</v>
       </c>
@@ -9792,7 +9796,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="201" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="201" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
         <v>3</v>
       </c>
@@ -9839,7 +9843,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="202" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="202" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
         <v>3</v>
       </c>
@@ -9886,7 +9890,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="203" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="203" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
         <v>3</v>
       </c>
@@ -9933,7 +9937,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="204" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="204" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
         <v>3</v>
       </c>
@@ -9980,7 +9984,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="205" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="205" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
         <v>3</v>
       </c>
@@ -10027,7 +10031,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="206" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="206" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
         <v>3</v>
       </c>
@@ -10074,7 +10078,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="207" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="207" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
         <v>3</v>
       </c>
@@ -10121,7 +10125,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="208" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="208" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
         <v>3</v>
       </c>
@@ -10168,7 +10172,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="209" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="209" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
         <v>3</v>
       </c>
@@ -10215,7 +10219,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="210" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="210" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
         <v>3</v>
       </c>
@@ -10262,7 +10266,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="211" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="211" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
         <v>3</v>
       </c>
@@ -10309,7 +10313,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="212" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="212" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
         <v>3</v>
       </c>
@@ -10356,7 +10360,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="213" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="213" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
         <v>3</v>
       </c>
@@ -10403,7 +10407,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="214" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="214" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
         <v>3</v>
       </c>
@@ -10450,7 +10454,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="215" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="215" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
         <v>3</v>
       </c>
@@ -10497,7 +10501,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="216" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="216" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
         <v>3</v>
       </c>
@@ -10544,7 +10548,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="217" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="217" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
         <v>3</v>
       </c>
@@ -10591,7 +10595,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="218" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="218" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
         <v>3</v>
       </c>
@@ -10638,7 +10642,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="219" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="219" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
         <v>3</v>
       </c>
@@ -10685,7 +10689,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="220" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="220" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
         <v>3</v>
       </c>
@@ -10732,7 +10736,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="221" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="221" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A221" t="s">
         <v>3</v>
       </c>
@@ -10779,7 +10783,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="222" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="222" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A222" t="s">
         <v>3</v>
       </c>
@@ -10826,7 +10830,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="223" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="223" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
         <v>3</v>
       </c>
@@ -10873,7 +10877,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="224" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="224" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
         <v>3</v>
       </c>
@@ -10920,7 +10924,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="225" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="225" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A225" t="s">
         <v>3</v>
       </c>
@@ -10967,7 +10971,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="226" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="226" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A226" t="s">
         <v>3</v>
       </c>
@@ -11014,7 +11018,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="227" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="227" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A227" t="s">
         <v>3</v>
       </c>
@@ -11061,7 +11065,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="228" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="228" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A228" t="s">
         <v>3</v>
       </c>
@@ -11108,7 +11112,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="229" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="229" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A229" t="s">
         <v>3</v>
       </c>
@@ -11155,7 +11159,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="230" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="230" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A230" t="s">
         <v>3</v>
       </c>
@@ -11202,7 +11206,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="231" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="231" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A231" t="s">
         <v>3</v>
       </c>
@@ -11249,7 +11253,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="232" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="232" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A232" t="s">
         <v>3</v>
       </c>
@@ -11296,7 +11300,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="233" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="233" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A233" t="s">
         <v>3</v>
       </c>
@@ -11343,7 +11347,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="234" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="234" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A234" t="s">
         <v>3</v>
       </c>
@@ -11390,7 +11394,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="235" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="235" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A235" t="s">
         <v>3</v>
       </c>
@@ -11437,7 +11441,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="236" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="236" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A236" t="s">
         <v>3</v>
       </c>
@@ -11484,7 +11488,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="237" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="237" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A237" t="s">
         <v>3</v>
       </c>
@@ -11531,7 +11535,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="238" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="238" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A238" t="s">
         <v>3</v>
       </c>
@@ -11578,7 +11582,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="239" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="239" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A239" t="s">
         <v>3</v>
       </c>
@@ -11625,7 +11629,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="240" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="240" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A240" t="s">
         <v>3</v>
       </c>
@@ -11672,7 +11676,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="241" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="241" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A241" t="s">
         <v>3</v>
       </c>
@@ -11719,7 +11723,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="242" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="242" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A242" t="s">
         <v>3</v>
       </c>
@@ -11766,7 +11770,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="243" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="243" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A243" t="s">
         <v>3</v>
       </c>
@@ -11813,7 +11817,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="244" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="244" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A244" t="s">
         <v>3</v>
       </c>
@@ -11860,7 +11864,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="245" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="245" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A245" t="s">
         <v>3</v>
       </c>
@@ -11907,7 +11911,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="246" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="246" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A246" t="s">
         <v>3</v>
       </c>
@@ -11954,7 +11958,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="247" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="247" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A247" t="s">
         <v>3</v>
       </c>
@@ -12001,7 +12005,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="248" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="248" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A248" t="s">
         <v>3</v>
       </c>
@@ -12048,7 +12052,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="249" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="249" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A249" t="s">
         <v>3</v>
       </c>
@@ -12095,7 +12099,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="250" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="250" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A250" t="s">
         <v>3</v>
       </c>
@@ -12142,7 +12146,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="251" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="251" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A251" t="s">
         <v>3</v>
       </c>
@@ -12189,7 +12193,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="252" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="252" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A252" t="s">
         <v>3</v>
       </c>
@@ -12236,7 +12240,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="253" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="253" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A253" t="s">
         <v>3</v>
       </c>
@@ -12283,7 +12287,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="254" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="254" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A254" t="s">
         <v>3</v>
       </c>
@@ -12330,7 +12334,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="255" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="255" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A255" t="s">
         <v>3</v>
       </c>
@@ -12377,7 +12381,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="256" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="256" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A256" t="s">
         <v>3</v>
       </c>
@@ -12430,17 +12434,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="8769bae9-3463-4a10-a579-45503be70aed" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="8dfbc409-28c6-489e-afb0-89cc2b931f2a">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -12449,7 +12442,7 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101008CB9B2C0AF3CE84CB4250F7CDCA74D24" ma:contentTypeVersion="11" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="2f42a97d5ab0c3bd2930341450d6f06b">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="8dfbc409-28c6-489e-afb0-89cc2b931f2a" xmlns:ns3="8769bae9-3463-4a10-a579-45503be70aed" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="dbd40f3811e35be07f3bce4a65cfcd28" ns2:_="" ns3:_="">
     <xsd:import namespace="8dfbc409-28c6-489e-afb0-89cc2b931f2a"/>
@@ -12644,18 +12637,18 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AFBD511E-5C1D-4223-BB26-D22E6EE722D3}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="8769bae9-3463-4a10-a579-45503be70aed"/>
-    <ds:schemaRef ds:uri="8dfbc409-28c6-489e-afb0-89cc2b931f2a"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="8769bae9-3463-4a10-a579-45503be70aed" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="8dfbc409-28c6-489e-afb0-89cc2b931f2a">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CE0CAF50-C050-48AE-875E-A3DE6E22B7B5}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
@@ -12663,7 +12656,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EE972C20-CF49-42CA-B59D-0D1129D9A052}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -12680,4 +12673,15 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AFBD511E-5C1D-4223-BB26-D22E6EE722D3}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="8769bae9-3463-4a10-a579-45503be70aed"/>
+    <ds:schemaRef ds:uri="8dfbc409-28c6-489e-afb0-89cc2b931f2a"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>